<commit_message>
Q1, partB3,4 hesaplamalar dışında tamamlandı
</commit_message>
<xml_diff>
--- a/Project1/B-H curve of core.xlsx
+++ b/Project1/B-H curve of core.xlsx
@@ -70,6 +70,242 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="tr-TR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>B</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t>(mT)-H(At/m)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t> curve</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sayfa1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sayfa1!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.440286624203821</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.414829332026784</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.777530504182334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.605900871220442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.808917197452232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.770700636942678</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.29543846104356</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.994150526452614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73.872217479808256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.593949044585983</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sayfa1!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>530</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="70152576"/>
+        <c:axId val="70154880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70152576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70154880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70154880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70152576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="3 Grafik"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -510,26 +746,31 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>510</v>
+        <v>520</v>
+      </c>
+      <c r="C13">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>510</v>
+        <v>530</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>510</v>
+        <v>530</v>
+      </c>
+      <c r="C15">
+        <v>1050</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>